<commit_message>
Add test case document template
</commit_message>
<xml_diff>
--- a/Documents/Workload/Milestone&WorkAssignment.xlsx
+++ b/Documents/Workload/Milestone&WorkAssignment.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Requirement ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,23 +165,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UnFinished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Event Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Processing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Processing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Processing</t>
+    <t>Finished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -311,13 +299,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -676,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -693,25 +681,25 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="16" thickBot="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -721,21 +709,21 @@
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" ht="16" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
@@ -743,25 +731,25 @@
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="16" thickBot="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -771,13 +759,13 @@
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
@@ -785,17 +773,17 @@
         <v>16</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="16" thickBot="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -805,13 +793,13 @@
         <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16" thickBot="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
@@ -819,17 +807,17 @@
         <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16" thickBot="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -839,13 +827,13 @@
         <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16" thickBot="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
@@ -853,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="31" thickBot="1">
@@ -873,11 +861,17 @@
         <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="G1:N3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -885,12 +879,6 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Package all for final paper
</commit_message>
<xml_diff>
--- a/Documents/Workload/Milestone&WorkAssignment.xlsx
+++ b/Documents/Workload/Milestone&WorkAssignment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>Requirement ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,7 +53,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>F00001</t>
+    <t>Nov.10 2013</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -61,23 +61,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>F00002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Shuai Zhao</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Nov.10 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F00003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F00004</t>
+    <t>Sprint Two</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nov.4 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprint Three</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No.11 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nov.17 2013</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -85,31 +89,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Sprint Four</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nov.18 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nov.24 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manual Document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Final Sprint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nov.25 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nov.30 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make up all document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jianghua Kuai&amp;Shuai Zhao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Shuai Zhao</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sprint Two</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nov.4 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprint Three</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No.11 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nov.17 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F00005</t>
+    <t>F00001 Client&amp;Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00002 Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -117,59 +149,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>F00007</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprint Four</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nov.18 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nov.24 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F00006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manual Document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Final Sprint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nov.25 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nov.30 2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Make up all document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jianghua Kuai&amp;Shuai Zhao</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>We'll use agile development method, so we'll release useable product every week. Every teammate will contribute to the product, so we assign the job by the requirements(also known as user story). Teammate should use unit test to test their code first.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Event Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished</t>
+    <t>Shuai Zhao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00002 Client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jianghua Kua</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00003 Client&amp;Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00004 Client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00004 Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00005 Client&amp;Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00007 Client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00007 Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jianghua Kuai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F00006 Client&amp;Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case Document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuai Zhao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workload and Milestone Sheet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -177,7 +209,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,6 +266,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -252,10 +293,29 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
       <top style="medium">
-        <color auto="1"/>
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -267,6 +327,61 @@
       <right style="medium">
         <color theme="4"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
       <top style="medium">
         <color theme="4"/>
       </top>
@@ -276,7 +391,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,39 +399,70 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -645,247 +791,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="36" customHeight="1" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="39" customHeight="1" thickBot="1">
+      <c r="A1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" ht="36" customHeight="1" thickBot="1">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1">
+      <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1">
+      <c r="A6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="16" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1">
-      <c r="A4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1">
+      <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="B9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1">
-      <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1">
-      <c r="A8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="31" thickBot="1">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" thickBot="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" thickBot="1">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16" thickBot="1">
+      <c r="A12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickBot="1">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="31" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="G1:N3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="80" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>